<commit_message>
+ Ajout d'une page utilisé afin de calibrer le capteur. [EN COURS]
</commit_message>
<xml_diff>
--- a/ressources/calculCaptTemp_1.xlsx
+++ b/ressources/calculCaptTemp_1.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educlgqc-my.sharepoint.com/personal/201770397_edu_clg_qc_ca/Documents/Projet-Final_1/doc_projet/ressources/outils/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\clg\Projet-Final\code\MOTRIK_capt-temperature\ressources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1256" documentId="8_{AF409BA0-701D-4870-91D0-EF5BD3536EE9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F52CB9C7-C591-4434-ACBA-118B40A93F50}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F2E031-D419-4DAC-8555-E83613C612C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7E244A9E-8CDC-43CC-8CF7-4099A6C94DF6}"/>
+    <workbookView xWindow="6240" yWindow="2760" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{7E244A9E-8CDC-43CC-8CF7-4099A6C94DF6}"/>
   </bookViews>
   <sheets>
     <sheet name="Calcul DE Temp. Max." sheetId="3" r:id="rId1"/>
     <sheet name="Calcul DE Ampli." sheetId="1" r:id="rId2"/>
     <sheet name="Calcul Range" sheetId="2" r:id="rId3"/>
+    <sheet name="Feuil1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,6 +42,30 @@
     <author>Thomas Desrosiers</author>
   </authors>
   <commentList>
+    <comment ref="H3" authorId="0" shapeId="0" xr:uid="{95EBB1DE-5F52-455E-9646-50BD12918A19}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Thomas Desrosiers:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Cette page est utilisé pour calculer la température maximale de la plage de mesure en température (Température minimale selon la datasheet jusqu'à une température calculée).</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B6" authorId="0" shapeId="0" xr:uid="{0DB3DB6E-3640-41FF-8D8B-087A536404DD}">
       <text>
         <r>
@@ -100,6 +125,30 @@
     <author>Thomas Desrosiers</author>
   </authors>
   <commentList>
+    <comment ref="I3" authorId="0" shapeId="0" xr:uid="{5C4E2621-BFDE-4711-B6F9-0FA78453EA87}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Thomas Desrosiers:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Cette page est utilisé pour calculer les paramètres d'amplification pour la plage de mesure en température (Température min. selon la datasheet jusqu'à une température max. choisie).</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B6" authorId="0" shapeId="0" xr:uid="{F22457A5-DD31-4DFD-8E1A-CEF65F4BC7C3}">
       <text>
         <r>
@@ -158,6 +207,30 @@
     <author>Thomas Desrosiers</author>
   </authors>
   <commentList>
+    <comment ref="K3" authorId="0" shapeId="0" xr:uid="{F8D1CEDF-BC75-480C-9108-017A70549E02}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Thomas Desrosiers:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Cette page est utilisé pour calculer les paramètres d'amplification et de décalage pour la plage de mesure en température (Température minimale choisie jusqu'à une température maximale choisie).</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B6" authorId="0" shapeId="0" xr:uid="{F46DBC5E-7A51-4903-9DDE-6F23778E49C6}">
       <text>
         <r>
@@ -211,7 +284,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="32">
   <si>
     <t>Temp. Min.</t>
   </si>
@@ -287,21 +360,41 @@
   <si>
     <t>Conversion valeur  ADC vers °C</t>
   </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>/1024</t>
+  </si>
+  <si>
+    <t>°C Réel</t>
+  </si>
+  <si>
+    <t>°C mesuré</t>
+  </si>
+  <si>
+    <t>tension</t>
+  </si>
+  <si>
+    <t>nouveau diviseur</t>
+  </si>
+  <si>
+    <t>diviseur</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="7">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="0.00&quot;mV/°C&quot;"/>
     <numFmt numFmtId="165" formatCode="0.00&quot;°C&quot;"/>
     <numFmt numFmtId="166" formatCode="0.00&quot;V&quot;"/>
     <numFmt numFmtId="167" formatCode="0&quot;bits&quot;"/>
     <numFmt numFmtId="168" formatCode="0.00&quot;kΩ&quot;"/>
-    <numFmt numFmtId="169" formatCode=";;;"/>
-    <numFmt numFmtId="171" formatCode="0.000&quot;V&quot;"/>
+    <numFmt numFmtId="169" formatCode="0.000&quot;V&quot;"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -348,8 +441,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Helvetica"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -374,6 +472,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="30">
     <border>
@@ -831,9 +935,6 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -978,24 +1079,150 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="4" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="6" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1006,129 +1233,6 @@
       <alignment horizontal="right" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="4" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="6" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="2"/>
     </xf>
   </cellXfs>
@@ -1136,28 +1240,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="36">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7F7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <bgColor rgb="FFFF7F7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <bgColor rgb="FFFF7F7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <fill>
         <patternFill patternType="lightUp">
@@ -1211,174 +1294,6 @@
       <fill>
         <patternFill patternType="lightUp">
           <bgColor rgb="FFFF7F7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7F7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <bgColor rgb="FFFF7F7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <bgColor rgb="FFFF7F7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7FFF7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7F7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <bgColor rgb="FFFF7F7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <bgColor rgb="FFFF7F7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7FFF7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7F7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <bgColor rgb="FFFF7F7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <bgColor rgb="FFFF7F7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <bgColor rgb="FFFF7F7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <bgColor rgb="FFFF7F7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7FFF7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7F7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7FFF7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7F7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <bgColor rgb="FFFF7F7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <bgColor rgb="FFFF7F7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <bgColor rgb="FFFF7F7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <bgColor rgb="FFFF7F7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7FFF7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7F7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7FFF7F"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1539,7 +1454,7 @@
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:filteredCategoryTitle>
                 <c15:cat>
-                  <c:numRef>
+                  <c:multiLvlStrRef>
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
@@ -1547,7 +1462,7 @@
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
-                  </c:numRef>
+                  </c:multiLvlStrRef>
                 </c15:cat>
               </c15:filteredCategoryTitle>
             </c:ext>
@@ -1603,7 +1518,7 @@
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:filteredCategoryTitle>
                 <c15:cat>
-                  <c:numRef>
+                  <c:multiLvlStrRef>
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
@@ -1611,7 +1526,7 @@
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
-                  </c:numRef>
+                  </c:multiLvlStrRef>
                 </c15:cat>
               </c15:filteredCategoryTitle>
             </c:ext>
@@ -3981,282 +3896,270 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{261590FB-39DA-4895-9B3E-8A7D443B4B53}">
   <dimension ref="B1:H26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="0.28515625" style="4" customWidth="1"/>
     <col min="2" max="2" width="29.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" style="91" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="0.5703125" style="99" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" style="78" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="0.5703125" style="86" customWidth="1"/>
     <col min="5" max="5" width="33.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.7109375" style="91" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.7109375" style="78" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.85546875" style="4" customWidth="1"/>
+    <col min="8" max="8" width="3" style="4" customWidth="1"/>
     <col min="9" max="9" width="0.7109375" style="4" customWidth="1"/>
     <col min="10" max="16384" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="1.5" customHeight="1" thickBot="1"/>
     <row r="2" spans="2:8" ht="15" customHeight="1" thickBot="1">
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="109" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
+      <c r="C2" s="110"/>
+      <c r="D2" s="60"/>
+      <c r="G2" s="60"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" thickBot="1">
       <c r="B3" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="38">
+      <c r="C3" s="37">
         <v>1024</v>
       </c>
-      <c r="D3" s="62"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="6"/>
+      <c r="D3" s="61"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="106" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="4" spans="2:8" ht="15" customHeight="1" thickBot="1">
       <c r="B4" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="39">
+      <c r="C4" s="38">
         <v>5</v>
       </c>
-      <c r="D4" s="50"/>
-      <c r="E4" s="72" t="s">
+      <c r="D4" s="49"/>
+      <c r="E4" s="109" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="73"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="6"/>
+      <c r="F4" s="110"/>
+      <c r="G4" s="54"/>
     </row>
     <row r="5" spans="2:8" ht="15" customHeight="1" thickBot="1">
-      <c r="D5" s="92"/>
-      <c r="G5" s="56"/>
-      <c r="H5" s="6"/>
+      <c r="D5" s="79"/>
+      <c r="G5" s="55"/>
     </row>
     <row r="6" spans="2:8" ht="15" customHeight="1" thickBot="1">
-      <c r="B6" s="72" t="s">
+      <c r="B6" s="109" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="73"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="72" t="s">
+      <c r="C6" s="110"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="109" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="73"/>
+      <c r="F6" s="110"/>
       <c r="G6" s="22"/>
-      <c r="H6" s="6"/>
     </row>
     <row r="7" spans="2:8" ht="15" customHeight="1" thickBot="1">
       <c r="B7" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="40">
+      <c r="C7" s="39">
         <v>10</v>
       </c>
-      <c r="D7" s="63"/>
+      <c r="D7" s="62"/>
       <c r="E7" s="9" t="str">
         <f>"Amplification " &amp;C20&amp; "V -&gt; " &amp;C4&amp; "V"</f>
-        <v>Amplification 1,5V -&gt; 5V</v>
-      </c>
-      <c r="F7" s="101">
+        <v>Amplification 1V -&gt; 5V</v>
+      </c>
+      <c r="F7" s="88">
         <v>4</v>
       </c>
       <c r="G7" s="5"/>
-      <c r="H7" s="6"/>
     </row>
     <row r="8" spans="2:8" ht="15" customHeight="1">
       <c r="B8" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="41">
+      <c r="C8" s="40">
         <v>0</v>
       </c>
-      <c r="D8" s="65"/>
+      <c r="D8" s="64"/>
       <c r="E8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="87">
+      <c r="F8" s="74">
         <f>C7*F7</f>
         <v>40</v>
       </c>
       <c r="G8" s="5"/>
-      <c r="H8" s="6"/>
     </row>
     <row r="9" spans="2:8" ht="15" customHeight="1">
       <c r="B9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="42">
+      <c r="C9" s="41">
         <v>150</v>
       </c>
-      <c r="D9" s="65"/>
+      <c r="D9" s="64"/>
       <c r="E9" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F9" s="46">
+      <c r="F9" s="45">
         <f>C8</f>
         <v>0</v>
       </c>
-      <c r="G9" s="61"/>
-      <c r="H9" s="61"/>
+      <c r="G9" s="60"/>
     </row>
     <row r="10" spans="2:8" ht="15" customHeight="1" thickBot="1">
       <c r="B10" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="43">
+      <c r="C10" s="42">
         <f>ABS(C9)+ABS(C8)</f>
         <v>150</v>
       </c>
-      <c r="D10" s="65"/>
+      <c r="D10" s="64"/>
       <c r="E10" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="46">
+      <c r="F10" s="45">
         <f>IF((C4/(F8*10^-3))&lt;=C10,C4/(F8*10^-3),C10)</f>
         <v>125</v>
       </c>
-      <c r="G10" s="61"/>
-      <c r="H10" s="61"/>
+      <c r="G10" s="60"/>
     </row>
     <row r="11" spans="2:8" ht="15" customHeight="1">
       <c r="B11" s="18" t="str">
         <f>"Tension @ " &amp;C8&amp; "°C"</f>
         <v>Tension @ 0°C</v>
       </c>
-      <c r="C11" s="44">
+      <c r="C11" s="43">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="D11" s="50"/>
+      <c r="D11" s="49"/>
       <c r="E11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="46">
+      <c r="F11" s="45">
         <f>F10+ABS(F9)</f>
         <v>125</v>
       </c>
-      <c r="G11" s="57"/>
-      <c r="H11" s="6"/>
+      <c r="G11" s="56"/>
     </row>
     <row r="12" spans="2:8" ht="15" customHeight="1" thickBot="1">
-      <c r="B12" s="90" t="str">
+      <c r="B12" s="77" t="str">
         <f>"Tension @ " &amp;C9&amp; "°C"</f>
         <v>Tension @ 150°C</v>
       </c>
-      <c r="C12" s="35">
+      <c r="C12" s="34">
         <f>C10*(C7*10^-3)</f>
         <v>1.5</v>
       </c>
-      <c r="D12" s="50"/>
+      <c r="D12" s="49"/>
       <c r="E12" s="3" t="str">
         <f>"Tension @ " &amp;F9&amp; "°C"</f>
         <v>Tension @ 0°C</v>
       </c>
-      <c r="F12" s="47">
+      <c r="F12" s="46">
         <f>C11</f>
         <v>0</v>
       </c>
-      <c r="G12" s="59"/>
-      <c r="H12" s="6"/>
+      <c r="G12" s="58"/>
     </row>
     <row r="13" spans="2:8" ht="15" customHeight="1" thickBot="1">
-      <c r="B13" s="58"/>
-      <c r="C13" s="50"/>
-      <c r="D13" s="50"/>
+      <c r="B13" s="57"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
       <c r="E13" s="3" t="str">
         <f>"Tension @ " &amp;ROUND(F10,2)&amp; "°C"</f>
         <v>Tension @ 125°C</v>
       </c>
-      <c r="F13" s="47">
+      <c r="F13" s="46">
         <f>F10*(F8*10^-3)</f>
         <v>5</v>
       </c>
-      <c r="G13" s="59"/>
-      <c r="H13" s="6"/>
+      <c r="G13" s="58"/>
     </row>
     <row r="14" spans="2:8" ht="15" customHeight="1" thickBot="1">
-      <c r="B14" s="72" t="s">
+      <c r="B14" s="109" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="73"/>
-      <c r="D14" s="61"/>
+      <c r="C14" s="110"/>
+      <c r="D14" s="60"/>
       <c r="E14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F14" s="47">
+      <c r="F14" s="46">
         <f>F13-F12</f>
         <v>5</v>
       </c>
-      <c r="G14" s="30"/>
-      <c r="H14" s="6"/>
+      <c r="G14" s="29"/>
     </row>
     <row r="15" spans="2:8" ht="15" customHeight="1" thickBot="1">
       <c r="B15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="100">
+      <c r="C15" s="87">
         <v>0</v>
       </c>
-      <c r="D15" s="65"/>
-      <c r="E15" s="102" t="s">
+      <c r="D15" s="64"/>
+      <c r="E15" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="F15" s="103">
+      <c r="F15" s="90">
         <f>F14/C4</f>
         <v>1</v>
       </c>
       <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
     </row>
     <row r="16" spans="2:8" ht="15" customHeight="1" thickBot="1">
       <c r="B16" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="42">
-        <v>150</v>
-      </c>
-      <c r="D16" s="65"/>
-      <c r="E16" s="104"/>
-      <c r="F16" s="69"/>
+      <c r="C16" s="41">
+        <v>100</v>
+      </c>
+      <c r="D16" s="64"/>
+      <c r="E16" s="91"/>
+      <c r="F16" s="68"/>
       <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
     </row>
     <row r="17" spans="2:6" ht="15" customHeight="1" thickBot="1">
       <c r="B17" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="46">
+      <c r="C17" s="45">
         <f>ABS(C16)+ABS(C15)</f>
-        <v>150</v>
-      </c>
-      <c r="D17" s="65"/>
-      <c r="E17" s="84" t="s">
+        <v>100</v>
+      </c>
+      <c r="D17" s="64"/>
+      <c r="E17" s="107" t="s">
         <v>15</v>
       </c>
-      <c r="F17" s="85"/>
+      <c r="F17" s="108"/>
     </row>
     <row r="18" spans="2:6" ht="15" customHeight="1">
       <c r="B18" s="3" t="str">
         <f>"Tension @ " &amp;C15&amp; "°C"</f>
         <v>Tension @ 0°C</v>
       </c>
-      <c r="C18" s="47">
+      <c r="C18" s="46">
         <f>ABS( (ABS(C15)-ABS(C8)))*(C7*10^-3)</f>
         <v>0</v>
       </c>
-      <c r="D18" s="50"/>
+      <c r="D18" s="49"/>
       <c r="E18" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="36">
+      <c r="F18" s="35">
         <f>F7-1</f>
         <v>3</v>
       </c>
@@ -4264,17 +4167,17 @@
     <row r="19" spans="2:6" ht="15" customHeight="1">
       <c r="B19" s="3" t="str">
         <f>"Tension @ " &amp;ROUND(C16,2)&amp; "°C"</f>
-        <v>Tension @ 150°C</v>
-      </c>
-      <c r="C19" s="34">
+        <v>Tension @ 100°C</v>
+      </c>
+      <c r="C19" s="33">
         <f>(C16+ABS(C8))*(C7*10^-3)</f>
-        <v>1.5</v>
-      </c>
-      <c r="D19" s="50"/>
+        <v>1</v>
+      </c>
+      <c r="D19" s="49"/>
       <c r="E19" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F19" s="32">
+      <c r="F19" s="31">
         <v>10</v>
       </c>
     </row>
@@ -4282,72 +4185,72 @@
       <c r="B20" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="34">
+      <c r="C20" s="33">
         <f>C19-C18</f>
-        <v>1.5</v>
-      </c>
-      <c r="D20" s="50"/>
+        <v>1</v>
+      </c>
+      <c r="D20" s="49"/>
       <c r="E20" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F20" s="32">
+      <c r="F20" s="31">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="2:6" ht="15" customHeight="1" thickBot="1">
-      <c r="B21" s="105" t="s">
+      <c r="B21" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="103">
+      <c r="C21" s="90">
         <f>C19/C4</f>
-        <v>0.3</v>
-      </c>
-      <c r="D21" s="69"/>
+        <v>0.2</v>
+      </c>
+      <c r="D21" s="68"/>
       <c r="E21" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F21" s="37">
+      <c r="F21" s="36">
         <f>(F19/F20)+1</f>
         <v>11</v>
       </c>
     </row>
     <row r="22" spans="2:6" ht="15" customHeight="1" thickBot="1">
-      <c r="B22" s="54"/>
-      <c r="C22" s="69"/>
-      <c r="D22" s="69"/>
+      <c r="B22" s="53"/>
+      <c r="C22" s="68"/>
+      <c r="D22" s="68"/>
     </row>
     <row r="23" spans="2:6" ht="15.75" thickBot="1">
       <c r="D23" s="6"/>
-      <c r="E23" s="84" t="s">
+      <c r="E23" s="107" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="85"/>
+      <c r="F23" s="108"/>
     </row>
     <row r="24" spans="2:6">
-      <c r="E24" s="83" t="str">
+      <c r="E24" s="72" t="str">
         <f>"Tension @ " &amp;ROUND(F10,2)&amp; "°C"</f>
         <v>Tension @ 125°C</v>
       </c>
-      <c r="F24" s="44">
+      <c r="F24" s="43">
         <f>F10*(F8*10^-3)</f>
         <v>5</v>
       </c>
     </row>
     <row r="25" spans="2:6">
-      <c r="E25" s="82" t="str">
+      <c r="E25" s="71" t="str">
         <f>"Valeur lue par l'ADC ( " &amp;C3&amp; "bits )"</f>
         <v>Valeur lue par l'ADC ( 1024bits )</v>
       </c>
-      <c r="F25" s="94">
+      <c r="F25" s="81">
         <f>(F24/C4)*C3</f>
         <v>1024</v>
       </c>
     </row>
     <row r="26" spans="2:6" ht="15.75" thickBot="1">
-      <c r="E26" s="98" t="s">
+      <c r="E26" s="85" t="s">
         <v>24</v>
       </c>
-      <c r="F26" s="96">
+      <c r="F26" s="83">
         <f>ROUND(F25/F10,2)</f>
         <v>8.19</v>
       </c>
@@ -4363,16 +4266,16 @@
     <mergeCell ref="E6:F6"/>
   </mergeCells>
   <conditionalFormatting sqref="F21">
-    <cfRule type="expression" dxfId="0" priority="9">
+    <cfRule type="expression" dxfId="8" priority="9">
       <formula>$F$21&lt;&gt;$F$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="7" priority="1">
+      <formula>$C$16&lt;$C$8</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="2">
       <formula>$C$16&gt;$C$9</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>$C$16&lt;$C$8</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4415,81 +4318,82 @@
   <dimension ref="B1:I48"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I21" sqref="I20:I21"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="0.28515625" style="4" customWidth="1"/>
     <col min="2" max="2" width="29.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" style="91" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" style="78" customWidth="1"/>
     <col min="4" max="4" width="0.7109375" style="4" customWidth="1"/>
     <col min="5" max="5" width="33.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" style="91" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="78" customWidth="1"/>
     <col min="7" max="7" width="13.5703125" style="4" customWidth="1"/>
     <col min="8" max="8" width="0.7109375" style="4" customWidth="1"/>
-    <col min="9" max="16384" width="11.42578125" style="4"/>
+    <col min="9" max="9" width="3" style="4" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="1.5" customHeight="1" thickBot="1"/>
     <row r="2" spans="2:9" ht="15" customHeight="1" thickBot="1">
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="109" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="G2" s="61"/>
+      <c r="C2" s="110"/>
+      <c r="G2" s="60"/>
     </row>
     <row r="3" spans="2:9" ht="15" customHeight="1" thickBot="1">
       <c r="B3" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="38">
+      <c r="C3" s="37">
         <v>1024</v>
       </c>
-      <c r="G3" s="30"/>
-      <c r="I3" s="23" t="b">
-        <v>1</v>
+      <c r="G3" s="29"/>
+      <c r="I3" s="106" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="15" customHeight="1" thickBot="1">
       <c r="B4" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="39">
+      <c r="C4" s="38">
         <v>5</v>
       </c>
-      <c r="E4" s="72" t="s">
+      <c r="E4" s="109" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="73"/>
-      <c r="G4" s="55"/>
+      <c r="F4" s="110"/>
+      <c r="G4" s="54"/>
     </row>
     <row r="5" spans="2:9" ht="15" customHeight="1" thickBot="1">
-      <c r="G5" s="56"/>
+      <c r="G5" s="55"/>
     </row>
     <row r="6" spans="2:9" ht="15" customHeight="1" thickBot="1">
-      <c r="B6" s="72" t="s">
+      <c r="B6" s="109" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="73"/>
-      <c r="E6" s="72" t="s">
+      <c r="C6" s="110"/>
+      <c r="E6" s="109" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="73"/>
+      <c r="F6" s="110"/>
       <c r="G6" s="22"/>
     </row>
     <row r="7" spans="2:9" ht="15" customHeight="1" thickBot="1">
       <c r="B7" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="40">
+      <c r="C7" s="39">
         <v>10</v>
       </c>
-      <c r="E7" s="86" t="str">
+      <c r="E7" s="73" t="str">
         <f>"Amplification " &amp;C20&amp; "V -&gt; " &amp;F18&amp; "V"</f>
-        <v>Amplification 1V -&gt; 3,33V</v>
-      </c>
-      <c r="F7" s="97">
+        <v>Amplification 1V -&gt; 5V</v>
+      </c>
+      <c r="F7" s="84">
         <f>ROUND(C4/C20,2)</f>
         <v>5</v>
       </c>
@@ -4499,13 +4403,13 @@
       <c r="B8" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="41">
+      <c r="C8" s="40">
         <v>0</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="87">
+      <c r="F8" s="74">
         <f>C7*F7</f>
         <v>50</v>
       </c>
@@ -4515,23 +4419,23 @@
       <c r="B9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="42">
+      <c r="C9" s="41">
         <v>100</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="46">
+      <c r="F9" s="45">
         <f>C4/(F8*10^-3)</f>
         <v>100</v>
       </c>
-      <c r="G9" s="66"/>
+      <c r="G9" s="65"/>
     </row>
     <row r="10" spans="2:9" ht="15" customHeight="1" thickBot="1">
       <c r="B10" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="43">
+      <c r="C10" s="42">
         <f>ABS(C9)+ABS(C8)</f>
         <v>100</v>
       </c>
@@ -4539,81 +4443,81 @@
         <f>"Tension @ " &amp;C15&amp; "°C"</f>
         <v>Tension @ 0°C</v>
       </c>
-      <c r="F10" s="47">
+      <c r="F10" s="46">
         <f>C15*(F8*10^-3)</f>
         <v>0</v>
       </c>
-      <c r="G10" s="66"/>
+      <c r="G10" s="65"/>
     </row>
     <row r="11" spans="2:9" ht="15" customHeight="1" thickBot="1">
       <c r="B11" s="18" t="str">
         <f>"Tension @ " &amp;C8&amp; "°C"</f>
         <v>Tension @ 0°C</v>
       </c>
-      <c r="C11" s="44">
+      <c r="C11" s="43">
         <v>0</v>
       </c>
-      <c r="E11" s="26" t="str">
+      <c r="E11" s="25" t="str">
         <f>"Tension @ " &amp;C16&amp; "°C"</f>
         <v>Tension @ 100°C</v>
       </c>
-      <c r="F11" s="88">
+      <c r="F11" s="75">
         <f>C16*(F8*10^-3)</f>
         <v>5</v>
       </c>
-      <c r="G11" s="57"/>
+      <c r="G11" s="56"/>
       <c r="H11" s="7"/>
     </row>
     <row r="12" spans="2:9" ht="15" customHeight="1" thickBot="1">
-      <c r="B12" s="90" t="str">
+      <c r="B12" s="77" t="str">
         <f>"Tension @ " &amp;C9&amp; "°C"</f>
         <v>Tension @ 100°C</v>
       </c>
-      <c r="C12" s="35">
+      <c r="C12" s="34">
         <f>ABS(ABS(C9)+ABS(C8))*(C7*10^-3)</f>
         <v>1</v>
       </c>
       <c r="E12" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="103">
+      <c r="F12" s="90">
         <f>F11/C4</f>
         <v>1</v>
       </c>
-      <c r="G12" s="59"/>
+      <c r="G12" s="58"/>
       <c r="H12" s="7"/>
     </row>
     <row r="13" spans="2:9" ht="15" customHeight="1" thickBot="1">
-      <c r="B13" s="58"/>
-      <c r="C13" s="50"/>
-      <c r="G13" s="59"/>
+      <c r="B13" s="57"/>
+      <c r="C13" s="49"/>
+      <c r="G13" s="58"/>
       <c r="H13" s="7"/>
     </row>
     <row r="14" spans="2:9" ht="15" customHeight="1" thickBot="1">
-      <c r="B14" s="72" t="s">
+      <c r="B14" s="109" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="73"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="84" t="s">
+      <c r="C14" s="110"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="107" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="85"/>
-      <c r="G14" s="30"/>
+      <c r="F14" s="108"/>
+      <c r="G14" s="29"/>
       <c r="H14" s="7"/>
     </row>
     <row r="15" spans="2:9" ht="15" customHeight="1">
       <c r="B15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="100">
+      <c r="C15" s="87">
         <f>C8</f>
         <v>0</v>
       </c>
       <c r="E15" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="36">
+      <c r="F15" s="35">
         <f>ROUND(F7-1,2)</f>
         <v>4</v>
       </c>
@@ -4624,33 +4528,33 @@
       <c r="B16" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="42">
+      <c r="C16" s="41">
         <v>100</v>
       </c>
       <c r="E16" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="32">
-        <v>23.3</v>
-      </c>
-      <c r="G16" s="66"/>
+      <c r="F16" s="31">
+        <v>20</v>
+      </c>
+      <c r="G16" s="65"/>
       <c r="H16" s="7"/>
     </row>
     <row r="17" spans="2:8" ht="15" customHeight="1">
       <c r="B17" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="46">
+      <c r="C17" s="45">
         <f>C16-C15</f>
         <v>100</v>
       </c>
       <c r="E17" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F17" s="32">
-        <v>10</v>
-      </c>
-      <c r="G17" s="66"/>
+      <c r="F17" s="31">
+        <v>5</v>
+      </c>
+      <c r="G17" s="65"/>
       <c r="H17" s="7"/>
     </row>
     <row r="18" spans="2:8" ht="15" customHeight="1" thickBot="1">
@@ -4658,16 +4562,16 @@
         <f>"Tension @ " &amp;C15&amp; "°C"</f>
         <v>Tension @ 0°C</v>
       </c>
-      <c r="C18" s="47">
+      <c r="C18" s="46">
         <f>ABS(ABS(C15)-ABS(C8))*(C7*10^-3)</f>
         <v>0</v>
       </c>
       <c r="E18" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="37">
+      <c r="F18" s="36">
         <f>ROUND((F16/F17)+1,2)</f>
-        <v>3.33</v>
+        <v>5</v>
       </c>
       <c r="G18" s="22"/>
       <c r="H18" s="7"/>
@@ -4677,42 +4581,42 @@
         <f>"Tension @ " &amp;C16&amp; "°C"</f>
         <v>Tension @ 100°C</v>
       </c>
-      <c r="C19" s="34">
+      <c r="C19" s="33">
         <f>ABS(ABS(C16)+ABS(C8))*(C7*10^-3)</f>
         <v>1</v>
       </c>
       <c r="D19" s="8"/>
-      <c r="G19" s="71"/>
+      <c r="G19" s="70"/>
       <c r="H19" s="7"/>
     </row>
     <row r="20" spans="2:8" ht="15" customHeight="1" thickBot="1">
       <c r="B20" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="34">
+      <c r="C20" s="33">
         <f>C19-C18</f>
         <v>1</v>
       </c>
-      <c r="E20" s="89" t="s">
+      <c r="E20" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="F20" s="109"/>
-      <c r="G20" s="71"/>
+      <c r="F20" s="96"/>
+      <c r="G20" s="70"/>
       <c r="H20" s="7"/>
     </row>
     <row r="21" spans="2:8" ht="15" customHeight="1" thickBot="1">
       <c r="B21" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="103">
+      <c r="C21" s="90">
         <f>C19/C4</f>
         <v>0.2</v>
       </c>
-      <c r="E21" s="83" t="str">
+      <c r="E21" s="72" t="str">
         <f>"Tension @ " &amp;ROUND(C16,2)&amp; "°C"</f>
         <v>Tension @ 100°C</v>
       </c>
-      <c r="F21" s="44">
+      <c r="F21" s="43">
         <f>C16*(F8*10^-3)</f>
         <v>5</v>
       </c>
@@ -4721,12 +4625,12 @@
     </row>
     <row r="22" spans="2:8" ht="15" customHeight="1">
       <c r="B22" s="15"/>
-      <c r="C22" s="69"/>
-      <c r="E22" s="82" t="str">
+      <c r="C22" s="68"/>
+      <c r="E22" s="71" t="str">
         <f>"Valeur lue par l'ADC ( " &amp;B25&amp; "bits )"</f>
         <v>Valeur lue par l'ADC ( bits )</v>
       </c>
-      <c r="F22" s="94">
+      <c r="F22" s="81">
         <f>(F21/C4)*C3</f>
         <v>1024</v>
       </c>
@@ -4734,11 +4638,11 @@
       <c r="H22" s="7"/>
     </row>
     <row r="23" spans="2:8" ht="15" customHeight="1" thickBot="1">
-      <c r="E23" s="98" t="str">
+      <c r="E23" s="85" t="str">
         <f>"Conversion Valeur " &amp;C3&amp; " vers °C"</f>
         <v>Conversion Valeur 1024 vers °C</v>
       </c>
-      <c r="F23" s="96">
+      <c r="F23" s="83">
         <f>F22/C16</f>
         <v>10.24</v>
       </c>
@@ -4753,187 +4657,187 @@
       <c r="G25" s="6"/>
     </row>
     <row r="26" spans="2:8" ht="15" customHeight="1">
-      <c r="B26" s="27"/>
-      <c r="C26" s="62"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="61"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
-      <c r="F26" s="92"/>
+      <c r="F26" s="79"/>
       <c r="G26" s="6"/>
     </row>
     <row r="27" spans="2:8" ht="15" customHeight="1">
-      <c r="B27" s="27"/>
-      <c r="C27" s="50"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="49"/>
       <c r="D27" s="6"/>
-      <c r="E27" s="61"/>
-      <c r="F27" s="93"/>
+      <c r="E27" s="60"/>
+      <c r="F27" s="80"/>
       <c r="G27" s="6"/>
     </row>
     <row r="28" spans="2:8" ht="15" customHeight="1">
       <c r="B28" s="6"/>
-      <c r="C28" s="92"/>
+      <c r="C28" s="79"/>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
-      <c r="F28" s="92"/>
+      <c r="F28" s="79"/>
       <c r="G28" s="6"/>
     </row>
     <row r="29" spans="2:8" ht="15" customHeight="1">
-      <c r="B29" s="61"/>
-      <c r="C29" s="93"/>
+      <c r="B29" s="60"/>
+      <c r="C29" s="80"/>
       <c r="D29" s="6"/>
-      <c r="E29" s="61"/>
-      <c r="F29" s="93"/>
+      <c r="E29" s="60"/>
+      <c r="F29" s="80"/>
       <c r="G29" s="6"/>
     </row>
     <row r="30" spans="2:8" ht="15" customHeight="1">
-      <c r="B30" s="27"/>
-      <c r="C30" s="63"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="62"/>
       <c r="D30" s="6"/>
-      <c r="E30" s="54"/>
-      <c r="F30" s="64"/>
+      <c r="E30" s="53"/>
+      <c r="F30" s="63"/>
       <c r="G30" s="6"/>
     </row>
     <row r="31" spans="2:8" ht="15" customHeight="1">
-      <c r="B31" s="27"/>
-      <c r="C31" s="65"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="64"/>
       <c r="D31" s="6"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="63"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="62"/>
       <c r="G31" s="6"/>
     </row>
     <row r="32" spans="2:8" ht="15" customHeight="1">
-      <c r="B32" s="27"/>
-      <c r="C32" s="65"/>
+      <c r="B32" s="26"/>
+      <c r="C32" s="64"/>
       <c r="D32" s="6"/>
-      <c r="E32" s="27"/>
-      <c r="F32" s="65"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="64"/>
       <c r="G32" s="6"/>
     </row>
     <row r="33" spans="2:7" ht="15" customHeight="1">
-      <c r="B33" s="27"/>
-      <c r="C33" s="65"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="64"/>
       <c r="D33" s="6"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="50"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="49"/>
       <c r="G33" s="6"/>
     </row>
     <row r="34" spans="2:7" ht="15" customHeight="1">
-      <c r="B34" s="29"/>
-      <c r="C34" s="50"/>
+      <c r="B34" s="28"/>
+      <c r="C34" s="49"/>
       <c r="D34" s="6"/>
-      <c r="E34" s="29"/>
-      <c r="F34" s="50"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="49"/>
       <c r="G34" s="6"/>
     </row>
     <row r="35" spans="2:7" ht="15" customHeight="1">
-      <c r="B35" s="58"/>
-      <c r="C35" s="50"/>
+      <c r="B35" s="57"/>
+      <c r="C35" s="49"/>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
-      <c r="F35" s="92"/>
+      <c r="F35" s="79"/>
       <c r="G35" s="6"/>
     </row>
     <row r="36" spans="2:7" ht="15" customHeight="1">
-      <c r="B36" s="58"/>
-      <c r="C36" s="50"/>
+      <c r="B36" s="57"/>
+      <c r="C36" s="49"/>
       <c r="D36" s="6"/>
-      <c r="E36" s="66"/>
-      <c r="F36" s="95"/>
+      <c r="E36" s="65"/>
+      <c r="F36" s="82"/>
       <c r="G36" s="6"/>
     </row>
     <row r="37" spans="2:7" ht="15" customHeight="1">
       <c r="B37" s="6"/>
-      <c r="C37" s="92"/>
-      <c r="D37" s="29"/>
-      <c r="E37" s="66"/>
-      <c r="F37" s="95"/>
+      <c r="C37" s="79"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="65"/>
+      <c r="F37" s="82"/>
       <c r="G37" s="6"/>
     </row>
     <row r="38" spans="2:7" ht="15" customHeight="1">
-      <c r="B38" s="61"/>
-      <c r="C38" s="93"/>
+      <c r="B38" s="60"/>
+      <c r="C38" s="80"/>
       <c r="D38" s="6"/>
-      <c r="E38" s="54"/>
-      <c r="F38" s="67"/>
+      <c r="E38" s="53"/>
+      <c r="F38" s="66"/>
       <c r="G38" s="6"/>
     </row>
     <row r="39" spans="2:7" ht="15" customHeight="1">
-      <c r="B39" s="27"/>
-      <c r="C39" s="65"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="64"/>
       <c r="D39" s="6"/>
-      <c r="E39" s="54"/>
-      <c r="F39" s="68"/>
+      <c r="E39" s="53"/>
+      <c r="F39" s="67"/>
       <c r="G39" s="6"/>
     </row>
     <row r="40" spans="2:7" ht="15" customHeight="1">
-      <c r="B40" s="27"/>
-      <c r="C40" s="65"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="64"/>
       <c r="D40" s="6"/>
-      <c r="E40" s="54"/>
-      <c r="F40" s="68"/>
+      <c r="E40" s="53"/>
+      <c r="F40" s="67"/>
       <c r="G40" s="6"/>
     </row>
     <row r="41" spans="2:7" ht="15" customHeight="1">
-      <c r="B41" s="27"/>
-      <c r="C41" s="65"/>
+      <c r="B41" s="26"/>
+      <c r="C41" s="64"/>
       <c r="D41" s="6"/>
-      <c r="E41" s="29"/>
-      <c r="F41" s="64"/>
+      <c r="E41" s="28"/>
+      <c r="F41" s="63"/>
       <c r="G41" s="6"/>
     </row>
     <row r="42" spans="2:7" ht="15" customHeight="1">
-      <c r="B42" s="29"/>
-      <c r="C42" s="50"/>
+      <c r="B42" s="28"/>
+      <c r="C42" s="49"/>
       <c r="D42" s="8"/>
       <c r="E42" s="6"/>
-      <c r="F42" s="92"/>
+      <c r="F42" s="79"/>
       <c r="G42" s="6"/>
     </row>
     <row r="43" spans="2:7" ht="15" customHeight="1">
-      <c r="B43" s="29"/>
-      <c r="C43" s="50"/>
+      <c r="B43" s="28"/>
+      <c r="C43" s="49"/>
       <c r="D43" s="6"/>
-      <c r="E43" s="66"/>
-      <c r="F43" s="95"/>
+      <c r="E43" s="65"/>
+      <c r="F43" s="82"/>
       <c r="G43" s="6"/>
     </row>
     <row r="44" spans="2:7" ht="15" customHeight="1">
-      <c r="B44" s="27"/>
-      <c r="C44" s="50"/>
+      <c r="B44" s="26"/>
+      <c r="C44" s="49"/>
       <c r="D44" s="6"/>
-      <c r="E44" s="66"/>
-      <c r="F44" s="95"/>
+      <c r="E44" s="65"/>
+      <c r="F44" s="82"/>
       <c r="G44" s="6"/>
     </row>
     <row r="45" spans="2:7" ht="15" customHeight="1">
-      <c r="B45" s="60"/>
-      <c r="C45" s="69"/>
+      <c r="B45" s="59"/>
+      <c r="C45" s="68"/>
       <c r="D45" s="6"/>
-      <c r="E45" s="29"/>
-      <c r="F45" s="50"/>
+      <c r="E45" s="28"/>
+      <c r="F45" s="49"/>
       <c r="G45" s="6"/>
     </row>
     <row r="46" spans="2:7" ht="15" customHeight="1">
-      <c r="B46" s="60"/>
-      <c r="C46" s="69"/>
+      <c r="B46" s="59"/>
+      <c r="C46" s="68"/>
       <c r="D46" s="6"/>
-      <c r="E46" s="70"/>
-      <c r="F46" s="92"/>
+      <c r="E46" s="69"/>
+      <c r="F46" s="79"/>
       <c r="G46" s="6"/>
     </row>
     <row r="47" spans="2:7" ht="15" customHeight="1">
       <c r="B47" s="6"/>
-      <c r="C47" s="92"/>
+      <c r="C47" s="79"/>
       <c r="D47" s="6"/>
-      <c r="E47" s="70"/>
-      <c r="F47" s="92"/>
+      <c r="E47" s="69"/>
+      <c r="F47" s="79"/>
       <c r="G47" s="6"/>
     </row>
     <row r="48" spans="2:7" ht="15" customHeight="1">
       <c r="B48" s="6"/>
-      <c r="C48" s="92"/>
+      <c r="C48" s="79"/>
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
-      <c r="F48" s="92"/>
+      <c r="F48" s="79"/>
       <c r="G48" s="6"/>
     </row>
   </sheetData>
@@ -4946,16 +4850,16 @@
     <mergeCell ref="E6:F6"/>
   </mergeCells>
   <conditionalFormatting sqref="F18">
-    <cfRule type="expression" dxfId="8" priority="7">
+    <cfRule type="expression" dxfId="5" priority="7">
       <formula>$F$18&lt;&gt;$F$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="expression" dxfId="7" priority="2">
+    <cfRule type="expression" dxfId="4" priority="1">
+      <formula>$C$16&lt;$C$8</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>$C$16&gt;$C$9</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="1">
-      <formula>$C$16&lt;$C$8</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4969,143 +4873,148 @@
   <dimension ref="B1:L28"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="0.28515625" style="4" customWidth="1"/>
     <col min="2" max="2" width="29.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" style="91" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" style="78" customWidth="1"/>
     <col min="4" max="4" width="0.7109375" style="4" customWidth="1"/>
     <col min="5" max="5" width="29.7109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" style="91" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" style="78" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="0.7109375" style="4" customWidth="1"/>
     <col min="8" max="8" width="23.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" style="91" customWidth="1"/>
-    <col min="10" max="16384" width="11.42578125" style="4"/>
+    <col min="9" max="9" width="14.28515625" style="78" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" style="4"/>
+    <col min="11" max="11" width="3" style="4" customWidth="1"/>
+    <col min="12" max="16384" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="1.5" customHeight="1" thickBot="1"/>
-    <row r="2" spans="2:9" ht="15" customHeight="1" thickBot="1">
-      <c r="B2" s="72" t="s">
+    <row r="1" spans="2:11" ht="1.5" customHeight="1" thickBot="1"/>
+    <row r="2" spans="2:11" ht="15" customHeight="1" thickBot="1">
+      <c r="B2" s="109" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="73"/>
-    </row>
-    <row r="3" spans="2:9" ht="15" customHeight="1" thickBot="1">
+      <c r="C2" s="110"/>
+    </row>
+    <row r="3" spans="2:11" ht="15" customHeight="1" thickBot="1">
       <c r="B3" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="38">
+      <c r="C3" s="37">
         <v>1024</v>
       </c>
-    </row>
-    <row r="4" spans="2:9" ht="15" customHeight="1" thickBot="1">
+      <c r="K3" s="106" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="15" customHeight="1" thickBot="1">
       <c r="B4" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="39">
+      <c r="C4" s="38">
         <v>5</v>
       </c>
-      <c r="E4" s="72" t="s">
+      <c r="E4" s="109" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="73"/>
-      <c r="H4" s="72" t="s">
+      <c r="F4" s="110"/>
+      <c r="H4" s="109" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="73"/>
-    </row>
-    <row r="5" spans="2:9" ht="3.75" customHeight="1" thickBot="1"/>
-    <row r="6" spans="2:9" ht="15" customHeight="1" thickBot="1">
-      <c r="B6" s="72" t="s">
+      <c r="I4" s="110"/>
+    </row>
+    <row r="5" spans="2:11" ht="3.75" customHeight="1" thickBot="1"/>
+    <row r="6" spans="2:11" ht="15" customHeight="1" thickBot="1">
+      <c r="B6" s="109" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="73"/>
-      <c r="E6" s="72" t="s">
+      <c r="C6" s="110"/>
+      <c r="E6" s="109" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="73"/>
-      <c r="H6" s="72" t="s">
+      <c r="F6" s="110"/>
+      <c r="H6" s="109" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="73"/>
-    </row>
-    <row r="7" spans="2:9" ht="15" customHeight="1" thickBot="1">
+      <c r="I6" s="110"/>
+    </row>
+    <row r="7" spans="2:11" ht="15" customHeight="1" thickBot="1">
       <c r="B7" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="40">
+      <c r="C7" s="39">
         <v>10</v>
       </c>
       <c r="E7" s="20" t="str">
         <f>"Amplification " &amp;C21&amp; "V -&gt; " &amp;F18&amp; "V"</f>
         <v>Amplification 0,4V -&gt; 5V</v>
       </c>
-      <c r="F7" s="52">
+      <c r="F7" s="51">
         <f>C4/C21</f>
         <v>12.5</v>
       </c>
-      <c r="H7" s="28" t="s">
+      <c r="H7" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="51">
+      <c r="I7" s="50">
         <f>$C$4-$F$11</f>
         <v>-7.5</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="15" customHeight="1">
+    <row r="8" spans="2:11" ht="15" customHeight="1">
       <c r="B8" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="41">
+      <c r="C8" s="40">
         <v>0</v>
       </c>
       <c r="E8" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="53">
+      <c r="F8" s="52">
         <f>C7*F7</f>
         <v>125</v>
       </c>
-      <c r="H8" s="120" t="str">
+      <c r="H8" s="103" t="str">
         <f>"Tension @ " &amp;$C$16&amp; "°C"</f>
         <v>Tension @ 60°C</v>
       </c>
-      <c r="I8" s="121">
+      <c r="I8" s="104">
         <f>$F$10+$I$7</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="15" customHeight="1" thickBot="1">
+    <row r="9" spans="2:11" ht="15" customHeight="1" thickBot="1">
       <c r="B9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="42">
+      <c r="C9" s="41">
         <v>100</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="33">
+      <c r="F9" s="32">
         <f>C4/(F8*10^-3)</f>
         <v>40</v>
       </c>
-      <c r="H9" s="118" t="str">
+      <c r="H9" s="101" t="str">
         <f>"Tension @ " &amp;$C$17&amp; "°C"</f>
         <v>Tension @ 100°C</v>
       </c>
-      <c r="I9" s="122">
+      <c r="I9" s="105">
         <f>$F$11+$I$7</f>
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="2:9" ht="15" customHeight="1" thickBot="1">
+    <row r="10" spans="2:11" ht="15" customHeight="1" thickBot="1">
       <c r="B10" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="43">
+      <c r="C10" s="42">
         <f>ABS(C9)+ABS(C8)</f>
         <v>100</v>
       </c>
@@ -5113,102 +5022,102 @@
         <f>"Tension @ " &amp;$C$16&amp; "°C"</f>
         <v>Tension @ 60°C</v>
       </c>
-      <c r="F10" s="34">
+      <c r="F10" s="33">
         <f>$C$19*$F$7</f>
         <v>7.5</v>
       </c>
       <c r="G10" s="7"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="49"/>
-    </row>
-    <row r="11" spans="2:9" ht="15" customHeight="1" thickBot="1">
+      <c r="H10" s="23"/>
+      <c r="I10" s="48"/>
+    </row>
+    <row r="11" spans="2:11" ht="15" customHeight="1" thickBot="1">
       <c r="B11" s="18" t="str">
         <f>"Tension @ " &amp;C8&amp; "°C"</f>
         <v>Tension @ 0°C</v>
       </c>
-      <c r="C11" s="44">
+      <c r="C11" s="43">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="E11" s="26" t="str">
+      <c r="E11" s="25" t="str">
         <f>"Tension @ " &amp;$C$17&amp; "°C"</f>
         <v>Tension @ 100°C</v>
       </c>
-      <c r="F11" s="35">
+      <c r="F11" s="34">
         <f>$C$20*$F$7</f>
         <v>12.5</v>
       </c>
       <c r="G11" s="7"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="50"/>
-    </row>
-    <row r="12" spans="2:9" ht="3.75" customHeight="1" thickBot="1">
-      <c r="B12" s="78" t="str">
+      <c r="H11" s="28"/>
+      <c r="I11" s="49"/>
+    </row>
+    <row r="12" spans="2:11" ht="3.75" customHeight="1" thickBot="1">
+      <c r="B12" s="119" t="str">
         <f>"Tension @ " &amp;C9&amp; "°C"</f>
         <v>Tension @ 100°C</v>
       </c>
-      <c r="C12" s="80">
+      <c r="C12" s="121">
         <f>ABS(ABS(C9)+ABS(C8))*(C7*10^-3)</f>
         <v>1</v>
       </c>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="2:9" ht="12" customHeight="1" thickBot="1">
-      <c r="B13" s="79"/>
-      <c r="C13" s="81"/>
-      <c r="E13" s="76" t="s">
+    <row r="13" spans="2:11" ht="12" customHeight="1" thickBot="1">
+      <c r="B13" s="120"/>
+      <c r="C13" s="122"/>
+      <c r="E13" s="115" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="74"/>
+      <c r="F13" s="116"/>
       <c r="G13" s="7"/>
-      <c r="H13" s="110" t="s">
+      <c r="H13" s="111" t="s">
         <v>15</v>
       </c>
-      <c r="I13" s="111"/>
-    </row>
-    <row r="14" spans="2:9" ht="3.75" customHeight="1" thickBot="1">
-      <c r="E14" s="77"/>
-      <c r="F14" s="75"/>
+      <c r="I13" s="112"/>
+    </row>
+    <row r="14" spans="2:11" ht="3.75" customHeight="1" thickBot="1">
+      <c r="E14" s="117"/>
+      <c r="F14" s="118"/>
       <c r="G14" s="7"/>
-      <c r="H14" s="112"/>
-      <c r="I14" s="113"/>
-    </row>
-    <row r="15" spans="2:9" ht="15" customHeight="1" thickBot="1">
-      <c r="B15" s="72" t="s">
+      <c r="H14" s="113"/>
+      <c r="I14" s="114"/>
+    </row>
+    <row r="15" spans="2:11" ht="15" customHeight="1" thickBot="1">
+      <c r="B15" s="109" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="73"/>
+      <c r="C15" s="110"/>
       <c r="E15" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="36">
+      <c r="F15" s="35">
         <f>F7-1</f>
         <v>11.5</v>
       </c>
       <c r="G15" s="7"/>
-      <c r="H15" s="114" t="s">
+      <c r="H15" s="97" t="s">
         <v>14</v>
       </c>
-      <c r="I15" s="115"/>
-    </row>
-    <row r="16" spans="2:9" ht="15" customHeight="1">
+      <c r="I15" s="98"/>
+    </row>
+    <row r="16" spans="2:11" ht="15" customHeight="1">
       <c r="B16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="45">
+      <c r="C16" s="44">
         <v>60</v>
       </c>
       <c r="E16" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="32">
+      <c r="F16" s="31">
         <v>4</v>
       </c>
       <c r="G16" s="7"/>
-      <c r="H16" s="116" t="s">
+      <c r="H16" s="99" t="s">
         <v>11</v>
       </c>
-      <c r="I16" s="117">
+      <c r="I16" s="100">
         <v>4</v>
       </c>
     </row>
@@ -5216,20 +5125,20 @@
       <c r="B17" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="42">
+      <c r="C17" s="41">
         <v>100</v>
       </c>
       <c r="E17" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F17" s="32">
+      <c r="F17" s="31">
         <v>1</v>
       </c>
       <c r="G17" s="7"/>
-      <c r="H17" s="116" t="s">
+      <c r="H17" s="99" t="s">
         <v>12</v>
       </c>
-      <c r="I17" s="117">
+      <c r="I17" s="100">
         <v>1</v>
       </c>
     </row>
@@ -5237,22 +5146,22 @@
       <c r="B18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="46">
+      <c r="C18" s="45">
         <f>C17-C16</f>
         <v>40</v>
       </c>
       <c r="E18" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="37">
+      <c r="F18" s="36">
         <f>(F16/F17)+1</f>
         <v>5</v>
       </c>
       <c r="G18" s="7"/>
-      <c r="H18" s="118" t="s">
+      <c r="H18" s="101" t="s">
         <v>13</v>
       </c>
-      <c r="I18" s="119">
+      <c r="I18" s="102">
         <f>(I16/I17)+1</f>
         <v>5</v>
       </c>
@@ -5262,12 +5171,12 @@
         <f>"Tension @ " &amp;$C$16&amp; "°C"</f>
         <v>Tension @ 60°C</v>
       </c>
-      <c r="C19" s="108">
+      <c r="C19" s="95">
         <f>C16*($C$7*10^-3)</f>
         <v>0.6</v>
       </c>
       <c r="E19" s="8"/>
-      <c r="F19" s="106"/>
+      <c r="F19" s="93"/>
       <c r="G19" s="7"/>
     </row>
     <row r="20" spans="2:12" ht="15" customHeight="1">
@@ -5275,7 +5184,7 @@
         <f>"Tension @ " &amp;$C$17&amp; "°C"</f>
         <v>Tension @ 100°C</v>
       </c>
-      <c r="C20" s="107">
+      <c r="C20" s="94">
         <f>C17*($C$7*10^-3)</f>
         <v>1</v>
       </c>
@@ -5285,7 +5194,7 @@
       <c r="B21" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="107">
+      <c r="C21" s="94">
         <f>C20-C19</f>
         <v>0.4</v>
       </c>
@@ -5295,78 +5204,71 @@
       <c r="B22" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="48">
+      <c r="C22" s="47">
         <f>C20/C4</f>
         <v>0.2</v>
       </c>
       <c r="G22" s="7"/>
-      <c r="I22" s="92"/>
+      <c r="I22" s="79"/>
       <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
       <c r="L22" s="6"/>
     </row>
     <row r="23" spans="2:12" ht="15" customHeight="1">
       <c r="B23" s="15"/>
-      <c r="C23" s="69"/>
-      <c r="I23" s="92"/>
+      <c r="C23" s="68"/>
+      <c r="I23" s="79"/>
       <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
       <c r="L23" s="6"/>
     </row>
     <row r="24" spans="2:12" ht="15" customHeight="1">
-      <c r="I24" s="92"/>
-      <c r="J24" s="31"/>
-      <c r="K24" s="6"/>
+      <c r="I24" s="79"/>
+      <c r="J24" s="30"/>
       <c r="L24" s="6"/>
     </row>
     <row r="25" spans="2:12" ht="15" customHeight="1">
-      <c r="I25" s="92"/>
+      <c r="I25" s="79"/>
       <c r="J25" s="5"/>
-      <c r="K25" s="6"/>
       <c r="L25" s="6"/>
     </row>
     <row r="26" spans="2:12" ht="15" customHeight="1">
-      <c r="I26" s="92"/>
+      <c r="I26" s="79"/>
       <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
       <c r="L26" s="6"/>
     </row>
     <row r="27" spans="2:12" ht="15" customHeight="1">
-      <c r="I27" s="92"/>
+      <c r="I27" s="79"/>
       <c r="J27" s="6"/>
-      <c r="K27" s="6"/>
       <c r="L27" s="6"/>
     </row>
     <row r="28" spans="2:12" ht="15" customHeight="1">
-      <c r="I28" s="92"/>
+      <c r="I28" s="79"/>
       <c r="J28" s="6"/>
-      <c r="K28" s="6"/>
       <c r="L28" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="E13:F14"/>
-    <mergeCell ref="E6:F6"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="B6:C6"/>
-    <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="H13:I14"/>
     <mergeCell ref="H6:I6"/>
+    <mergeCell ref="E13:F14"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E4:F4"/>
   </mergeCells>
   <conditionalFormatting sqref="F18">
-    <cfRule type="expression" dxfId="11" priority="6">
+    <cfRule type="expression" dxfId="2" priority="6">
       <formula>$F$18&lt;&gt;$F$10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16:C17">
-    <cfRule type="expression" dxfId="10" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>$C16&gt;$C$9</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>$C16&lt;$C$8</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5375,4 +5277,75 @@
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0BB7E9A-41C3-42BD-B8A0-9E9EFDE7672A}">
+  <dimension ref="H18:I25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="18" spans="8:9">
+      <c r="H18" t="s">
+        <v>28</v>
+      </c>
+      <c r="I18">
+        <v>23.5</v>
+      </c>
+    </row>
+    <row r="19" spans="8:9">
+      <c r="H19" t="s">
+        <v>31</v>
+      </c>
+      <c r="I19">
+        <v>11.17675</v>
+      </c>
+    </row>
+    <row r="20" spans="8:9">
+      <c r="H20" t="s">
+        <v>26</v>
+      </c>
+      <c r="I20">
+        <f>I18*I19</f>
+        <v>262.65362499999998</v>
+      </c>
+    </row>
+    <row r="21" spans="8:9">
+      <c r="H21" t="s">
+        <v>29</v>
+      </c>
+      <c r="I21">
+        <f>(I20/1024)*5</f>
+        <v>1.2824884033203123</v>
+      </c>
+    </row>
+    <row r="23" spans="8:9">
+      <c r="H23" t="s">
+        <v>27</v>
+      </c>
+      <c r="I23">
+        <v>29.5</v>
+      </c>
+    </row>
+    <row r="24" spans="8:9">
+      <c r="H24" t="s">
+        <v>30</v>
+      </c>
+      <c r="I24">
+        <f>I20/I23</f>
+        <v>8.9035127118644066</v>
+      </c>
+    </row>
+    <row r="25" spans="8:9">
+      <c r="I25">
+        <v>8.9035127118644066</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>